<commit_message>
Fix: update project journal
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -249,7 +249,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.83"/>
@@ -306,7 +306,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0.111111111111111</v>
+        <v>0.128472222222222</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Work: tests for PotenotTaskCalculatorImpl
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -432,11 +432,11 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -532,8 +532,18 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>45544</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4"/>
@@ -622,11 +632,11 @@
   </sheetPr>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -864,14 +874,30 @@
       <c r="M3" s="13" t="n">
         <v>224986</v>
       </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
+      <c r="N3" s="13" t="n">
+        <v>0.791317738</v>
+      </c>
+      <c r="O3" s="13" t="n">
+        <v>45.2021</v>
+      </c>
+      <c r="P3" s="13" t="n">
+        <v>1.579809013</v>
+      </c>
+      <c r="Q3" s="13" t="n">
+        <v>90.3059</v>
+      </c>
+      <c r="R3" s="13" t="n">
+        <v>625.62443</v>
+      </c>
+      <c r="S3" s="13" t="n">
+        <v>-1176.961644</v>
+      </c>
+      <c r="T3" s="13" t="n">
+        <v>152.0024</v>
+      </c>
+      <c r="U3" s="13" t="n">
+        <v>2.653017829</v>
+      </c>
       <c r="V3" s="13"/>
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
@@ -925,14 +951,26 @@
       <c r="M4" s="13" t="n">
         <v>1173462</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
+      <c r="N4" s="13" t="n">
+        <v>0.127026032</v>
+      </c>
+      <c r="O4" s="13" t="n">
+        <v>7.1641</v>
+      </c>
+      <c r="P4" s="13" t="n">
+        <v>0.151140665</v>
+      </c>
+      <c r="Q4" s="13" t="n">
+        <v>8.3935</v>
+      </c>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
+      <c r="T4" s="13" t="n">
+        <v>317.1807</v>
+      </c>
+      <c r="U4" s="13" t="n">
+        <v>5.537963654</v>
+      </c>
       <c r="V4" s="13"/>
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
@@ -986,14 +1024,26 @@
       <c r="M5" s="13" t="n">
         <v>742845</v>
       </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
+      <c r="N5" s="13" t="n">
+        <v>0.163236954</v>
+      </c>
+      <c r="O5" s="13" t="n">
+        <v>20.4843</v>
+      </c>
+      <c r="P5" s="13" t="n">
+        <v>0.754787027</v>
+      </c>
+      <c r="Q5" s="13" t="n">
+        <v>43.1446</v>
+      </c>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
+      <c r="T5" s="13" t="n">
+        <v>163.0559</v>
+      </c>
+      <c r="U5" s="13" t="n">
+        <v>2.846627162</v>
+      </c>
       <c r="V5" s="13"/>
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>

</xml_diff>

<commit_message>
Work: tests for potenot calculator
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -432,11 +432,11 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -546,8 +546,18 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>45547</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0.0590277777777778</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4"/>
@@ -630,13 +640,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC17" activeCellId="0" sqref="AC17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -898,12 +908,20 @@
       <c r="U3" s="13" t="n">
         <v>2.653017829</v>
       </c>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
+      <c r="V3" s="13" t="n">
+        <v>197.2045</v>
+      </c>
+      <c r="W3" s="13" t="n">
+        <v>3.444334557</v>
+      </c>
+      <c r="X3" s="13" t="n">
+        <v>242.3223</v>
+      </c>
+      <c r="Y3" s="13" t="n">
+        <v>4.232825831</v>
+      </c>
       <c r="Z3" s="13" t="n">
-        <v>18462</v>
+        <v>18514</v>
       </c>
       <c r="AA3" s="13" t="n">
         <v>143392</v>
@@ -963,26 +981,42 @@
       <c r="Q4" s="13" t="n">
         <v>8.3935</v>
       </c>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
+      <c r="R4" s="13" t="n">
+        <v>-630177.7442</v>
+      </c>
+      <c r="S4" s="13" t="n">
+        <v>683001.4427</v>
+      </c>
       <c r="T4" s="13" t="n">
-        <v>317.1807</v>
+        <v>317.1813</v>
       </c>
       <c r="U4" s="13" t="n">
-        <v>5.537963654</v>
-      </c>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
+        <v>5.537992742</v>
+      </c>
+      <c r="V4" s="13" t="n">
+        <v>324.3454</v>
+      </c>
+      <c r="W4" s="13" t="n">
+        <v>5.665018775</v>
+      </c>
+      <c r="X4" s="13" t="n">
+        <v>325.5748</v>
+      </c>
+      <c r="Y4" s="13" t="n">
+        <v>5.689133407</v>
+      </c>
       <c r="Z4" s="13" t="n">
-        <v>-708968</v>
-      </c>
-      <c r="AA4" s="13" t="n">
-        <v>846444</v>
-      </c>
+        <v>-709005</v>
+      </c>
+      <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
+      <c r="AE4" s="0" t="n">
+        <v>-709005</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <v>846434</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
@@ -1025,7 +1059,7 @@
         <v>742845</v>
       </c>
       <c r="N5" s="13" t="n">
-        <v>0.163236954</v>
+        <v>0.363236954</v>
       </c>
       <c r="O5" s="13" t="n">
         <v>20.4843</v>
@@ -1036,26 +1070,42 @@
       <c r="Q5" s="13" t="n">
         <v>43.1446</v>
       </c>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
+      <c r="R5" s="13" t="n">
+        <v>49548.54946</v>
+      </c>
+      <c r="S5" s="13" t="n">
+        <v>-163086.6288</v>
+      </c>
       <c r="T5" s="13" t="n">
-        <v>163.0559</v>
+        <v>163.0601</v>
       </c>
       <c r="U5" s="13" t="n">
-        <v>2.846627162</v>
-      </c>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
+        <v>2.846636858</v>
+      </c>
+      <c r="V5" s="13" t="n">
+        <v>183.5444</v>
+      </c>
+      <c r="W5" s="13" t="n">
+        <v>3.209873812</v>
+      </c>
+      <c r="X5" s="13" t="n">
+        <v>206.2047</v>
+      </c>
+      <c r="Y5" s="13" t="n">
+        <v>3.601423886</v>
+      </c>
       <c r="Z5" s="13" t="n">
-        <v>150297</v>
-      </c>
-      <c r="AA5" s="13" t="n">
-        <v>-176047</v>
-      </c>
+        <v>183368</v>
+      </c>
+      <c r="AA5" s="13"/>
       <c r="AB5" s="13"/>
       <c r="AC5" s="13"/>
+      <c r="AE5" s="0" t="n">
+        <v>15295</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <v>-176044</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>

</xml_diff>

<commit_message>
Work: sucсessful testing PotenotCalculatorImpl
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">all tasks</t>
   </si>
   <si>
-    <t xml:space="preserve">Разработка тестов для PotenotService</t>
+    <t xml:space="preserve">Разработка тестов для PotenotCalculatorImpl</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -432,11 +432,11 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -560,8 +560,18 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>45548</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.0138888888888889</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4"/>
@@ -640,13 +650,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC17" activeCellId="0" sqref="AC17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC6" activeCellId="0" sqref="AC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -924,7 +934,7 @@
         <v>18514</v>
       </c>
       <c r="AA3" s="13" t="n">
-        <v>143392</v>
+        <v>143314</v>
       </c>
       <c r="AB3" s="13"/>
       <c r="AC3" s="13"/>
@@ -1008,15 +1018,11 @@
       <c r="Z4" s="13" t="n">
         <v>-709005</v>
       </c>
-      <c r="AA4" s="13"/>
+      <c r="AA4" s="13" t="n">
+        <v>846434</v>
+      </c>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
-      <c r="AE4" s="0" t="n">
-        <v>-709005</v>
-      </c>
-      <c r="AF4" s="0" t="n">
-        <v>846434</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
@@ -1095,17 +1101,13 @@
         <v>3.601423886</v>
       </c>
       <c r="Z5" s="13" t="n">
-        <v>183368</v>
-      </c>
-      <c r="AA5" s="13"/>
+        <v>150295</v>
+      </c>
+      <c r="AA5" s="13" t="n">
+        <v>-176044</v>
+      </c>
       <c r="AB5" s="13"/>
       <c r="AC5" s="13"/>
-      <c r="AE5" s="0" t="n">
-        <v>15295</v>
-      </c>
-      <c r="AF5" s="0" t="n">
-        <v>-176044</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>

</xml_diff>

<commit_message>
Work: service layer tests
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">Разработка сервиса для решения обратной геодезической засечки</t>
   </si>
   <si>
-    <t xml:space="preserve">PotenotTaskServece</t>
+    <t xml:space="preserve">PotenotTaskService</t>
   </si>
   <si>
     <t xml:space="preserve">Оптимизация слоя DTO</t>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t xml:space="preserve">Разработка тестов для PotenotCalculatorImpl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разработка тестов для PotenotTaskMapperImpl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разработка тестов для слоя servise</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -433,10 +439,10 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -574,12 +580,32 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>45551</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>45551</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4"/>
@@ -650,13 +676,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC6" activeCellId="0" sqref="AC6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -682,96 +708,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="X1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="Z1" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="13" t="n">
         <v>100000</v>
@@ -853,10 +879,16 @@
       </c>
       <c r="AB2" s="13"/>
       <c r="AC2" s="13"/>
+      <c r="AE2" s="13" t="n">
+        <v>137114</v>
+      </c>
+      <c r="AF2" s="13" t="n">
+        <v>209238</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="13" t="n">
         <v>100000</v>
@@ -938,10 +970,16 @@
       </c>
       <c r="AB3" s="13"/>
       <c r="AC3" s="13"/>
+      <c r="AE3" s="0" t="n">
+        <v>18515</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>143314</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="13" t="n">
         <v>100000</v>
@@ -1023,10 +1061,16 @@
       </c>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
+      <c r="AE4" s="13" t="n">
+        <v>-709005</v>
+      </c>
+      <c r="AF4" s="13" t="n">
+        <v>846436</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="13" t="n">
         <v>-100000</v>
@@ -1108,6 +1152,12 @@
       </c>
       <c r="AB5" s="13"/>
       <c r="AC5" s="13"/>
+      <c r="AE5" s="13" t="n">
+        <v>150295</v>
+      </c>
+      <c r="AF5" s="13" t="n">
+        <v>-176044</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>
@@ -1612,13 +1662,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Work: swagger documentation developes
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t xml:space="preserve">Разработка сквозных тестов для слоя controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разработка swagger документации для API</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -552,10 +555,10 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -768,16 +771,24 @@
       <c r="C14" s="6" t="n">
         <v>0.0243055555555556</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>45559</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>0.0451388888888889</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -848,7 +859,7 @@
       <c r="B25" s="12"/>
       <c r="C25" s="13" t="n">
         <f aca="false">SUM(C2:C24)</f>
-        <v>1.23611111111111</v>
+        <v>1.28125</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="11"/>
@@ -884,7 +895,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -910,96 +921,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>21</v>
-      </c>
       <c r="J1" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="17" t="s">
-        <v>29</v>
-      </c>
       <c r="R1" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S1" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T1" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U1" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="17" t="s">
-        <v>34</v>
-      </c>
       <c r="X1" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Z1" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA1" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB1" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC1" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="19" t="n">
         <v>100000</v>
@@ -1090,7 +1101,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="19" t="n">
         <v>100000</v>
@@ -1181,7 +1192,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="19" t="n">
         <v>100000</v>
@@ -1272,7 +1283,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="19" t="n">
         <v>-100000</v>
@@ -1864,13 +1875,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,7 +1985,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -1988,37 +1999,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Feat: expantion of DirectTaskController
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t xml:space="preserve">Разработка swagger документации для API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Расширение DirectTaskController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DirectTask*</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -600,13 +606,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -849,60 +855,68 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13" t="n">
-        <f aca="false">SUM(C3:C16)</f>
-        <v>1.29513888888889</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="11"/>
+      <c r="B17" s="6" t="n">
+        <v>42014</v>
+      </c>
+      <c r="C17" s="7" t="n">
+        <v>0.0520833333333333</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13" t="n">
+        <f aca="false">SUM(C3:C17)</f>
+        <v>1.34722222222222</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="7" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
+      <c r="D22" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,25 +955,39 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="15"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="18"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="18"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="18"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A21:E21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -982,7 +1010,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1008,96 +1036,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>28</v>
-      </c>
       <c r="J1" s="20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="X1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="21" t="s">
-        <v>41</v>
-      </c>
       <c r="Z1" s="22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AA1" s="22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AB1" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AC1" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B2" s="23" t="n">
         <v>100000</v>
@@ -1188,7 +1216,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" s="23" t="n">
         <v>100000</v>
@@ -1279,7 +1307,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B4" s="23" t="n">
         <v>100000</v>
@@ -1370,7 +1398,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B5" s="23" t="n">
         <v>-100000</v>
@@ -1962,13 +1990,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,7 +2100,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2086,37 +2114,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Work: developes InverseTask components
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t xml:space="preserve">geocalculator_web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разработка InverseTask</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -235,11 +238,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="hh:mm"/>
-    <numFmt numFmtId="167" formatCode="[hh]:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="168" formatCode="[hh]:mm:ss"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -424,7 +428,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -485,6 +489,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -493,7 +501,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -621,10 +629,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -983,10 +991,18 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
+      <c r="A28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="15" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C28" s="7" t="n">
+        <v>0.0277777777777778</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,20 +1048,20 @@
       <c r="E34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="15"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="18"/>
+      <c r="C36" s="19"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="18"/>
+      <c r="C37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="18"/>
+      <c r="C38" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1073,7 +1089,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1098,269 +1114,269 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="I1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="K1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="M1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="O1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="21" t="s">
+      <c r="P1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="Q1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="S1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="T1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="U1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="X1" s="21" t="s">
+      <c r="V1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" s="22" t="s">
+      <c r="W1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="22" t="s">
+      <c r="Y1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" s="22" t="s">
+      <c r="AA1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" s="22" t="s">
+      <c r="AB1" s="23" t="s">
         <v>53</v>
       </c>
+      <c r="AC1" s="23" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="23" t="n">
+      <c r="A2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="24" t="n">
         <v>251.1405</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="24" t="n">
         <v>904445</v>
       </c>
-      <c r="F2" s="23" t="n">
+      <c r="F2" s="24" t="n">
         <v>200000</v>
       </c>
-      <c r="G2" s="23" t="n">
+      <c r="G2" s="24" t="n">
         <v>200000</v>
       </c>
-      <c r="H2" s="23" t="n">
+      <c r="H2" s="24" t="n">
         <v>351.3834</v>
       </c>
-      <c r="I2" s="23" t="n">
+      <c r="I2" s="24" t="n">
         <v>1265914</v>
       </c>
-      <c r="J2" s="23" t="n">
+      <c r="J2" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="K2" s="23" t="n">
+      <c r="K2" s="24" t="n">
         <v>300000</v>
       </c>
-      <c r="L2" s="23" t="n">
+      <c r="L2" s="24" t="n">
         <v>112.1425</v>
       </c>
-      <c r="M2" s="23" t="n">
+      <c r="M2" s="24" t="n">
         <v>404065</v>
       </c>
-      <c r="N2" s="23" t="n">
+      <c r="N2" s="24" t="n">
         <v>1.752451165</v>
       </c>
-      <c r="O2" s="23" t="n">
+      <c r="O2" s="24" t="n">
         <v>100.2429</v>
       </c>
-      <c r="P2" s="23" t="n">
+      <c r="P2" s="24" t="n">
         <v>3.85727461</v>
       </c>
-      <c r="Q2" s="23" t="n">
+      <c r="Q2" s="24" t="n">
         <v>221.002</v>
       </c>
-      <c r="R2" s="23" t="n">
+      <c r="R2" s="24" t="n">
         <v>-348396.5989</v>
       </c>
-      <c r="S2" s="23" t="n">
+      <c r="S2" s="24" t="n">
         <v>-118367.968</v>
       </c>
-      <c r="T2" s="23" t="n">
+      <c r="T2" s="24" t="n">
         <v>251.1405</v>
       </c>
-      <c r="U2" s="23" t="n">
+      <c r="U2" s="24" t="n">
         <v>4.384873098</v>
       </c>
-      <c r="V2" s="23" t="n">
+      <c r="V2" s="24" t="n">
         <v>351.3834</v>
       </c>
-      <c r="W2" s="23" t="n">
+      <c r="W2" s="24" t="n">
         <v>6.137324263</v>
       </c>
-      <c r="X2" s="23" t="n">
+      <c r="X2" s="24" t="n">
         <v>112.1425</v>
       </c>
-      <c r="Y2" s="23" t="n">
+      <c r="Y2" s="24" t="n">
         <v>1.958962401</v>
       </c>
-      <c r="Z2" s="23" t="n">
+      <c r="Z2" s="24" t="n">
         <v>137114</v>
       </c>
-      <c r="AA2" s="23" t="n">
+      <c r="AA2" s="24" t="n">
         <v>209238</v>
       </c>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AE2" s="23" t="n">
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AE2" s="24" t="n">
         <v>137114</v>
       </c>
-      <c r="AF2" s="23" t="n">
+      <c r="AF2" s="24" t="n">
         <v>209238</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="23" t="n">
+      <c r="A3" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="D3" s="23" t="n">
+      <c r="D3" s="24" t="n">
         <v>331.5847</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="24" t="n">
         <v>1195127</v>
       </c>
-      <c r="F3" s="23" t="n">
+      <c r="F3" s="24" t="n">
         <v>200000</v>
       </c>
-      <c r="G3" s="23" t="n">
+      <c r="G3" s="24" t="n">
         <v>200000</v>
       </c>
-      <c r="H3" s="23" t="n">
+      <c r="H3" s="24" t="n">
         <v>17.1908</v>
       </c>
-      <c r="I3" s="23" t="n">
+      <c r="I3" s="24" t="n">
         <v>62348</v>
       </c>
-      <c r="J3" s="23" t="n">
+      <c r="J3" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="K3" s="23" t="n">
+      <c r="K3" s="24" t="n">
         <v>300000</v>
       </c>
-      <c r="L3" s="23" t="n">
+      <c r="L3" s="24" t="n">
         <v>62.2946</v>
       </c>
-      <c r="M3" s="23" t="n">
+      <c r="M3" s="24" t="n">
         <v>224986</v>
       </c>
-      <c r="N3" s="23" t="n">
+      <c r="N3" s="24" t="n">
         <v>0.791317738</v>
       </c>
-      <c r="O3" s="23" t="n">
+      <c r="O3" s="24" t="n">
         <v>45.2021</v>
       </c>
-      <c r="P3" s="23" t="n">
+      <c r="P3" s="24" t="n">
         <v>1.579809013</v>
       </c>
-      <c r="Q3" s="23" t="n">
+      <c r="Q3" s="24" t="n">
         <v>90.3059</v>
       </c>
-      <c r="R3" s="23" t="n">
+      <c r="R3" s="24" t="n">
         <v>625.62443</v>
       </c>
-      <c r="S3" s="23" t="n">
+      <c r="S3" s="24" t="n">
         <v>-1176.961644</v>
       </c>
-      <c r="T3" s="23" t="n">
+      <c r="T3" s="24" t="n">
         <v>152.0024</v>
       </c>
-      <c r="U3" s="23" t="n">
+      <c r="U3" s="24" t="n">
         <v>2.653017829</v>
       </c>
-      <c r="V3" s="23" t="n">
+      <c r="V3" s="24" t="n">
         <v>197.2045</v>
       </c>
-      <c r="W3" s="23" t="n">
+      <c r="W3" s="24" t="n">
         <v>3.444334557</v>
       </c>
-      <c r="X3" s="23" t="n">
+      <c r="X3" s="24" t="n">
         <v>242.3223</v>
       </c>
-      <c r="Y3" s="23" t="n">
+      <c r="Y3" s="24" t="n">
         <v>4.232825831</v>
       </c>
-      <c r="Z3" s="23" t="n">
+      <c r="Z3" s="24" t="n">
         <v>18514</v>
       </c>
-      <c r="AA3" s="23" t="n">
+      <c r="AA3" s="24" t="n">
         <v>143314</v>
       </c>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
       <c r="AE3" s="0" t="n">
         <v>18515</v>
       </c>
@@ -1369,777 +1385,777 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="23" t="n">
+      <c r="A4" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="C4" s="23" t="n">
+      <c r="C4" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="D4" s="23" t="n">
+      <c r="D4" s="24" t="n">
         <v>317.1807</v>
       </c>
-      <c r="E4" s="23" t="n">
+      <c r="E4" s="24" t="n">
         <v>1142287</v>
       </c>
-      <c r="F4" s="23" t="n">
+      <c r="F4" s="24" t="n">
         <v>200000</v>
       </c>
-      <c r="G4" s="23" t="n">
+      <c r="G4" s="24" t="n">
         <v>200000</v>
       </c>
-      <c r="H4" s="23" t="n">
+      <c r="H4" s="24" t="n">
         <v>324.3448</v>
       </c>
-      <c r="I4" s="23" t="n">
+      <c r="I4" s="24" t="n">
         <v>1168488</v>
       </c>
-      <c r="J4" s="23" t="n">
+      <c r="J4" s="24" t="n">
         <v>100000</v>
       </c>
-      <c r="K4" s="23" t="n">
+      <c r="K4" s="24" t="n">
         <v>300000</v>
       </c>
-      <c r="L4" s="23" t="n">
+      <c r="L4" s="24" t="n">
         <v>325.5742</v>
       </c>
-      <c r="M4" s="23" t="n">
+      <c r="M4" s="24" t="n">
         <v>1173462</v>
       </c>
-      <c r="N4" s="23" t="n">
+      <c r="N4" s="24" t="n">
         <v>0.127026032</v>
       </c>
-      <c r="O4" s="23" t="n">
+      <c r="O4" s="24" t="n">
         <v>7.1641</v>
       </c>
-      <c r="P4" s="23" t="n">
+      <c r="P4" s="24" t="n">
         <v>0.151140665</v>
       </c>
-      <c r="Q4" s="23" t="n">
+      <c r="Q4" s="24" t="n">
         <v>8.3935</v>
       </c>
-      <c r="R4" s="23" t="n">
+      <c r="R4" s="24" t="n">
         <v>-630177.7442</v>
       </c>
-      <c r="S4" s="23" t="n">
+      <c r="S4" s="24" t="n">
         <v>683001.4427</v>
       </c>
-      <c r="T4" s="23" t="n">
+      <c r="T4" s="24" t="n">
         <v>317.1813</v>
       </c>
-      <c r="U4" s="23" t="n">
+      <c r="U4" s="24" t="n">
         <v>5.537992742</v>
       </c>
-      <c r="V4" s="23" t="n">
+      <c r="V4" s="24" t="n">
         <v>324.3454</v>
       </c>
-      <c r="W4" s="23" t="n">
+      <c r="W4" s="24" t="n">
         <v>5.665018775</v>
       </c>
-      <c r="X4" s="23" t="n">
+      <c r="X4" s="24" t="n">
         <v>325.5748</v>
       </c>
-      <c r="Y4" s="23" t="n">
+      <c r="Y4" s="24" t="n">
         <v>5.689133407</v>
       </c>
-      <c r="Z4" s="23" t="n">
+      <c r="Z4" s="24" t="n">
         <v>-709005</v>
       </c>
-      <c r="AA4" s="23" t="n">
+      <c r="AA4" s="24" t="n">
         <v>846434</v>
       </c>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AE4" s="23" t="n">
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AE4" s="24" t="n">
         <v>-709005</v>
       </c>
-      <c r="AF4" s="23" t="n">
+      <c r="AF4" s="24" t="n">
         <v>846436</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="23" t="n">
+      <c r="A5" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="24" t="n">
         <v>-100000</v>
       </c>
-      <c r="C5" s="23" t="n">
+      <c r="C5" s="24" t="n">
         <v>-100000</v>
       </c>
-      <c r="D5" s="23" t="n">
+      <c r="D5" s="24" t="n">
         <v>163.0559</v>
       </c>
-      <c r="E5" s="23" t="n">
+      <c r="E5" s="24" t="n">
         <v>587159</v>
       </c>
-      <c r="F5" s="23" t="n">
+      <c r="F5" s="24" t="n">
         <v>-200000</v>
       </c>
-      <c r="G5" s="23" t="n">
+      <c r="G5" s="24" t="n">
         <v>-200000</v>
       </c>
-      <c r="H5" s="23" t="n">
+      <c r="H5" s="24" t="n">
         <v>183.5442</v>
       </c>
-      <c r="I5" s="23" t="n">
+      <c r="I5" s="24" t="n">
         <v>662082</v>
       </c>
-      <c r="J5" s="23" t="n">
+      <c r="J5" s="24" t="n">
         <v>-100000</v>
       </c>
-      <c r="K5" s="23" t="n">
+      <c r="K5" s="24" t="n">
         <v>-300000</v>
       </c>
-      <c r="L5" s="23" t="n">
+      <c r="L5" s="24" t="n">
         <v>206.2045</v>
       </c>
-      <c r="M5" s="23" t="n">
+      <c r="M5" s="24" t="n">
         <v>742845</v>
       </c>
-      <c r="N5" s="23" t="n">
+      <c r="N5" s="24" t="n">
         <v>0.363236954</v>
       </c>
-      <c r="O5" s="23" t="n">
+      <c r="O5" s="24" t="n">
         <v>20.4843</v>
       </c>
-      <c r="P5" s="23" t="n">
+      <c r="P5" s="24" t="n">
         <v>0.754787027</v>
       </c>
-      <c r="Q5" s="23" t="n">
+      <c r="Q5" s="24" t="n">
         <v>43.1446</v>
       </c>
-      <c r="R5" s="23" t="n">
+      <c r="R5" s="24" t="n">
         <v>49548.54946</v>
       </c>
-      <c r="S5" s="23" t="n">
+      <c r="S5" s="24" t="n">
         <v>-163086.6288</v>
       </c>
-      <c r="T5" s="23" t="n">
+      <c r="T5" s="24" t="n">
         <v>163.0601</v>
       </c>
-      <c r="U5" s="23" t="n">
+      <c r="U5" s="24" t="n">
         <v>2.846636858</v>
       </c>
-      <c r="V5" s="23" t="n">
+      <c r="V5" s="24" t="n">
         <v>183.5444</v>
       </c>
-      <c r="W5" s="23" t="n">
+      <c r="W5" s="24" t="n">
         <v>3.209873812</v>
       </c>
-      <c r="X5" s="23" t="n">
+      <c r="X5" s="24" t="n">
         <v>206.2047</v>
       </c>
-      <c r="Y5" s="23" t="n">
+      <c r="Y5" s="24" t="n">
         <v>3.601423886</v>
       </c>
-      <c r="Z5" s="23" t="n">
+      <c r="Z5" s="24" t="n">
         <v>150295</v>
       </c>
-      <c r="AA5" s="23" t="n">
+      <c r="AA5" s="24" t="n">
         <v>-176044</v>
       </c>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
-      <c r="AE5" s="23" t="n">
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AE5" s="24" t="n">
         <v>150295</v>
       </c>
-      <c r="AF5" s="23" t="n">
+      <c r="AF5" s="24" t="n">
         <v>-176044</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="24"/>
+      <c r="AB7" s="24"/>
+      <c r="AC7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="23"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="23"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="24"/>
+      <c r="AC11" s="24"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="23"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="24"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="24"/>
+      <c r="Z13" s="24"/>
+      <c r="AA13" s="24"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="23"/>
-      <c r="AC14" s="23"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="24"/>
+      <c r="AC17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
-      <c r="AC18" s="23"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="24"/>
+      <c r="AB19" s="24"/>
+      <c r="AC19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="23"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="23"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="23"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="23"/>
-      <c r="AB21" s="23"/>
-      <c r="AC21" s="23"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G23" s="24" t="n">
+      <c r="G23" s="25" t="n">
         <v>1296000</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>58</v>
+      <c r="D24" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="25" t="n">
+      <c r="D25" s="26" t="n">
         <v>1265914</v>
       </c>
-      <c r="E25" s="25" t="n">
+      <c r="E25" s="26" t="n">
         <v>62348</v>
       </c>
-      <c r="F25" s="25" t="n">
+      <c r="F25" s="26" t="n">
         <v>92434</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="25" t="n">
+      <c r="D26" s="26" t="n">
         <v>62348</v>
       </c>
-      <c r="E26" s="25" t="n">
+      <c r="E26" s="26" t="n">
         <v>1265914</v>
       </c>
-      <c r="F26" s="25" t="n">
+      <c r="F26" s="26" t="n">
         <v>1203566</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="25" t="n">
+      <c r="D27" s="26" t="n">
         <v>1142287</v>
       </c>
-      <c r="E27" s="25" t="n">
+      <c r="E27" s="26" t="n">
         <v>587159</v>
       </c>
-      <c r="F27" s="25" t="n">
+      <c r="F27" s="26" t="n">
         <v>740872</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="25" t="n">
+      <c r="D28" s="26" t="n">
         <v>587159</v>
       </c>
-      <c r="E28" s="25" t="n">
+      <c r="E28" s="26" t="n">
         <v>1142287</v>
       </c>
-      <c r="F28" s="25" t="n">
+      <c r="F28" s="26" t="n">
         <v>555128</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2163,7 +2179,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2176,145 +2192,145 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="E1" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="G1" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="H1" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="I1" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="J1" s="28" t="s">
         <v>68</v>
       </c>
+      <c r="K1" s="28" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="n">
+      <c r="A2" s="29" t="n">
         <v>1000000000</v>
       </c>
-      <c r="B2" s="28" t="n">
+      <c r="B2" s="29" t="n">
         <v>1000000000</v>
       </c>
-      <c r="C2" s="28" t="n">
+      <c r="C2" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D2" s="28" t="n">
+      <c r="D2" s="29" t="n">
         <v>2000000000</v>
       </c>
-      <c r="E2" s="28" t="n">
+      <c r="E2" s="29" t="n">
         <v>2000000000</v>
       </c>
-      <c r="F2" s="28" t="n">
+      <c r="F2" s="29" t="n">
         <v>200000</v>
       </c>
-      <c r="G2" s="28" t="n">
+      <c r="G2" s="29" t="n">
         <v>162000</v>
       </c>
-      <c r="H2" s="28" t="n">
+      <c r="H2" s="29" t="n">
         <v>1414213562</v>
       </c>
-      <c r="I2" s="28" t="n">
+      <c r="I2" s="29" t="n">
         <v>1414213566</v>
       </c>
-      <c r="J2" s="28" t="n">
+      <c r="J2" s="29" t="n">
         <v>14</v>
       </c>
-      <c r="K2" s="28" t="n">
+      <c r="K2" s="29" t="n">
         <v>100000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="n">
+      <c r="A3" s="29" t="n">
         <v>2000000000</v>
       </c>
-      <c r="B3" s="28" t="n">
+      <c r="B3" s="29" t="n">
         <v>2000000000</v>
       </c>
-      <c r="C3" s="28" t="n">
+      <c r="C3" s="29" t="n">
         <v>200000</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Work: injectes thymeleaf add DataHandler, UiController
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t xml:space="preserve">InverseTask*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UiController, DataHandler, внедрение в проект thymeleaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UIController, DataHandler</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -634,11 +640,11 @@
   </sheetPr>
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -926,10 +932,18 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>45681</v>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>0.09375</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,12 +962,12 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="13" t="n">
         <f aca="false">SUM(C3:C22)</f>
-        <v>1.45138888888889</v>
+        <v>1.54513888888889</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="11"/>
@@ -974,7 +988,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -983,22 +997,22 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C27" s="7" t="n">
         <v>0.0416666666666667</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B28" s="15" t="n">
         <v>45678</v>
@@ -1007,13 +1021,13 @@
         <v>0.0277777777777778</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B29" s="15" t="n">
         <v>45679</v>
@@ -1022,7 +1036,7 @@
         <v>0.0381944444444444</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1103,7 +1117,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1129,96 +1143,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" s="21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="S1" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="T1" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U1" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V1" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="W1" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X1" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="22" t="s">
-        <v>50</v>
-      </c>
       <c r="Z1" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AA1" s="23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AC1" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" s="24" t="n">
         <v>100000</v>
@@ -1309,7 +1323,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3" s="24" t="n">
         <v>100000</v>
@@ -1400,7 +1414,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4" s="24" t="n">
         <v>100000</v>
@@ -1491,7 +1505,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B5" s="24" t="n">
         <v>-100000</v>
@@ -2083,13 +2097,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,7 +2207,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2207,37 +2221,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Feat: UiController is worked, all tests is ready
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t xml:space="preserve">UIController, DataHandler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataMapper, Validator, InverseStringResponse, InverseStringRequest, тесты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UiController, InverseServiceImplTest</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -638,17 +644,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.29"/>
   </cols>
   <sheetData>
@@ -947,10 +953,18 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="6" t="n">
+        <v>45684</v>
+      </c>
+      <c r="C21" s="7" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,16 +975,11 @@
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13" t="n">
-        <f aca="false">SUM(C3:C22)</f>
-        <v>1.54513888888889</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="11"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
@@ -980,78 +989,83 @@
       <c r="E24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13" t="n">
+        <f aca="false">SUM(C3:C24)</f>
+        <v>1.67013888888889</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="7" t="n">
-        <v>0.0416666666666667</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="15" t="n">
-        <v>45678</v>
-      </c>
-      <c r="C28" s="7" t="n">
-        <v>0.0277777777777778</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="7" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="15" t="n">
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="15" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C30" s="7" t="n">
+        <v>0.0277777777777778</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="15" t="n">
         <v>45679</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C31" s="7" t="n">
         <v>0.0381944444444444</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
+      <c r="D31" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="E31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,25 +1090,39 @@
       <c r="E34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="16"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="16"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="19"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="19"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="19"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="19"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A28:E28"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1117,7 +1145,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1143,96 +1171,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>39</v>
-      </c>
       <c r="J1" s="21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="S1" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="T1" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="U1" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="V1" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="W1" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="X1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="22" t="s">
-        <v>52</v>
-      </c>
       <c r="Z1" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AA1" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AC1" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" s="24" t="n">
         <v>100000</v>
@@ -1323,7 +1351,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B3" s="24" t="n">
         <v>100000</v>
@@ -1414,7 +1442,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B4" s="24" t="n">
         <v>100000</v>
@@ -1505,7 +1533,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5" s="24" t="n">
         <v>-100000</v>
@@ -2097,13 +2125,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2207,7 +2235,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2221,37 +2249,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Work: add PotenotStringRequest, PotenotStringResponse. Added methods to PotenotTaskMapper. Added tests to PotenotServiceImplTest
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t xml:space="preserve">Разработка тестов DirectTaskServiceImpIntegrationTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PotenotStringRequest, PotenotStringResponse. Расширение PotenotTaskMapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PotenotTask*</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -268,12 +274,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="hh:mm"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="168" formatCode="[hh]:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="hh:mm"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="169" formatCode="[hh]:mm:ss"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -458,7 +465,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,51 +482,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,11 +542,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -659,10 +670,10 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -1025,10 +1036,18 @@
       <c r="E24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
+      <c r="A25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>45691</v>
+      </c>
+      <c r="C25" s="7" t="n">
+        <v>0.0902777777777778</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="E25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,7 +1066,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="13" t="n">
@@ -1072,56 +1091,56 @@
       <c r="E30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="A31" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C32" s="7" t="n">
         <v>0.0416666666666667</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="15" t="n">
+        <v>40</v>
+      </c>
+      <c r="B33" s="16" t="n">
         <v>45678</v>
       </c>
       <c r="C33" s="7" t="n">
         <v>0.0277777777777778</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="15" t="n">
+        <v>41</v>
+      </c>
+      <c r="B34" s="16" t="n">
         <v>45679</v>
       </c>
       <c r="C34" s="7" t="n">
         <v>0.0381944444444444</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1161,20 +1180,20 @@
       <c r="E39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="16"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="17"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="19"/>
+      <c r="C41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="19"/>
+      <c r="C42" s="20"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="19"/>
+      <c r="C43" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1202,7 +1221,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1227,269 +1246,269 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="A1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="21" t="s">
+      <c r="G1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="H1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="I1" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="M1" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="22" t="s">
+      <c r="O1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="P1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="Q1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="S1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="22" t="s">
+      <c r="T1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="W1" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="X1" s="22" t="s">
+      <c r="U1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z1" s="23" t="s">
+      <c r="V1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="AA1" s="23" t="s">
+      <c r="W1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="AB1" s="23" t="s">
+      <c r="Y1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z1" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AA1" s="24" t="s">
         <v>64</v>
       </c>
+      <c r="AB1" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC1" s="24" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="24" t="n">
+      <c r="A2" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="C2" s="24" t="n">
+      <c r="C2" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="D2" s="24" t="n">
+      <c r="D2" s="25" t="n">
         <v>251.1405</v>
       </c>
-      <c r="E2" s="24" t="n">
+      <c r="E2" s="25" t="n">
         <v>904445</v>
       </c>
-      <c r="F2" s="24" t="n">
+      <c r="F2" s="25" t="n">
         <v>200000</v>
       </c>
-      <c r="G2" s="24" t="n">
+      <c r="G2" s="25" t="n">
         <v>200000</v>
       </c>
-      <c r="H2" s="24" t="n">
+      <c r="H2" s="25" t="n">
         <v>351.3834</v>
       </c>
-      <c r="I2" s="24" t="n">
+      <c r="I2" s="25" t="n">
         <v>1265914</v>
       </c>
-      <c r="J2" s="24" t="n">
+      <c r="J2" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="K2" s="24" t="n">
+      <c r="K2" s="25" t="n">
         <v>300000</v>
       </c>
-      <c r="L2" s="24" t="n">
+      <c r="L2" s="25" t="n">
         <v>112.1425</v>
       </c>
-      <c r="M2" s="24" t="n">
+      <c r="M2" s="25" t="n">
         <v>404065</v>
       </c>
-      <c r="N2" s="24" t="n">
+      <c r="N2" s="25" t="n">
         <v>1.752451165</v>
       </c>
-      <c r="O2" s="24" t="n">
+      <c r="O2" s="25" t="n">
         <v>100.2429</v>
       </c>
-      <c r="P2" s="24" t="n">
+      <c r="P2" s="25" t="n">
         <v>3.85727461</v>
       </c>
-      <c r="Q2" s="24" t="n">
+      <c r="Q2" s="25" t="n">
         <v>221.002</v>
       </c>
-      <c r="R2" s="24" t="n">
+      <c r="R2" s="25" t="n">
         <v>-348396.5989</v>
       </c>
-      <c r="S2" s="24" t="n">
+      <c r="S2" s="25" t="n">
         <v>-118367.968</v>
       </c>
-      <c r="T2" s="24" t="n">
+      <c r="T2" s="25" t="n">
         <v>251.1405</v>
       </c>
-      <c r="U2" s="24" t="n">
+      <c r="U2" s="25" t="n">
         <v>4.384873098</v>
       </c>
-      <c r="V2" s="24" t="n">
+      <c r="V2" s="25" t="n">
         <v>351.3834</v>
       </c>
-      <c r="W2" s="24" t="n">
+      <c r="W2" s="25" t="n">
         <v>6.137324263</v>
       </c>
-      <c r="X2" s="24" t="n">
+      <c r="X2" s="25" t="n">
         <v>112.1425</v>
       </c>
-      <c r="Y2" s="24" t="n">
+      <c r="Y2" s="25" t="n">
         <v>1.958962401</v>
       </c>
-      <c r="Z2" s="24" t="n">
+      <c r="Z2" s="25" t="n">
         <v>137114</v>
       </c>
-      <c r="AA2" s="24" t="n">
+      <c r="AA2" s="25" t="n">
         <v>209238</v>
       </c>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AE2" s="24" t="n">
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AE2" s="25" t="n">
         <v>137114</v>
       </c>
-      <c r="AF2" s="24" t="n">
+      <c r="AF2" s="25" t="n">
         <v>209238</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="24" t="n">
+      <c r="A3" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="C3" s="24" t="n">
+      <c r="C3" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="D3" s="24" t="n">
+      <c r="D3" s="25" t="n">
         <v>331.5847</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E3" s="25" t="n">
         <v>1195127</v>
       </c>
-      <c r="F3" s="24" t="n">
+      <c r="F3" s="25" t="n">
         <v>200000</v>
       </c>
-      <c r="G3" s="24" t="n">
+      <c r="G3" s="25" t="n">
         <v>200000</v>
       </c>
-      <c r="H3" s="24" t="n">
+      <c r="H3" s="25" t="n">
         <v>17.1908</v>
       </c>
-      <c r="I3" s="24" t="n">
+      <c r="I3" s="25" t="n">
         <v>62348</v>
       </c>
-      <c r="J3" s="24" t="n">
+      <c r="J3" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="K3" s="24" t="n">
+      <c r="K3" s="25" t="n">
         <v>300000</v>
       </c>
-      <c r="L3" s="24" t="n">
+      <c r="L3" s="25" t="n">
         <v>62.2946</v>
       </c>
-      <c r="M3" s="24" t="n">
+      <c r="M3" s="25" t="n">
         <v>224986</v>
       </c>
-      <c r="N3" s="24" t="n">
+      <c r="N3" s="25" t="n">
         <v>0.791317738</v>
       </c>
-      <c r="O3" s="24" t="n">
+      <c r="O3" s="25" t="n">
         <v>45.2021</v>
       </c>
-      <c r="P3" s="24" t="n">
+      <c r="P3" s="25" t="n">
         <v>1.579809013</v>
       </c>
-      <c r="Q3" s="24" t="n">
+      <c r="Q3" s="25" t="n">
         <v>90.3059</v>
       </c>
-      <c r="R3" s="24" t="n">
+      <c r="R3" s="25" t="n">
         <v>625.62443</v>
       </c>
-      <c r="S3" s="24" t="n">
+      <c r="S3" s="25" t="n">
         <v>-1176.961644</v>
       </c>
-      <c r="T3" s="24" t="n">
+      <c r="T3" s="25" t="n">
         <v>152.0024</v>
       </c>
-      <c r="U3" s="24" t="n">
+      <c r="U3" s="25" t="n">
         <v>2.653017829</v>
       </c>
-      <c r="V3" s="24" t="n">
+      <c r="V3" s="25" t="n">
         <v>197.2045</v>
       </c>
-      <c r="W3" s="24" t="n">
+      <c r="W3" s="25" t="n">
         <v>3.444334557</v>
       </c>
-      <c r="X3" s="24" t="n">
+      <c r="X3" s="25" t="n">
         <v>242.3223</v>
       </c>
-      <c r="Y3" s="24" t="n">
+      <c r="Y3" s="25" t="n">
         <v>4.232825831</v>
       </c>
-      <c r="Z3" s="24" t="n">
+      <c r="Z3" s="25" t="n">
         <v>18514</v>
       </c>
-      <c r="AA3" s="24" t="n">
+      <c r="AA3" s="25" t="n">
         <v>143314</v>
       </c>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
       <c r="AE3" s="0" t="n">
         <v>18515</v>
       </c>
@@ -1498,777 +1517,777 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="24" t="n">
+      <c r="A4" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="C4" s="24" t="n">
+      <c r="C4" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="D4" s="24" t="n">
+      <c r="D4" s="25" t="n">
         <v>317.1807</v>
       </c>
-      <c r="E4" s="24" t="n">
+      <c r="E4" s="25" t="n">
         <v>1142287</v>
       </c>
-      <c r="F4" s="24" t="n">
+      <c r="F4" s="25" t="n">
         <v>200000</v>
       </c>
-      <c r="G4" s="24" t="n">
+      <c r="G4" s="25" t="n">
         <v>200000</v>
       </c>
-      <c r="H4" s="24" t="n">
+      <c r="H4" s="25" t="n">
         <v>324.3448</v>
       </c>
-      <c r="I4" s="24" t="n">
+      <c r="I4" s="25" t="n">
         <v>1168488</v>
       </c>
-      <c r="J4" s="24" t="n">
+      <c r="J4" s="25" t="n">
         <v>100000</v>
       </c>
-      <c r="K4" s="24" t="n">
+      <c r="K4" s="25" t="n">
         <v>300000</v>
       </c>
-      <c r="L4" s="24" t="n">
+      <c r="L4" s="25" t="n">
         <v>325.5742</v>
       </c>
-      <c r="M4" s="24" t="n">
+      <c r="M4" s="25" t="n">
         <v>1173462</v>
       </c>
-      <c r="N4" s="24" t="n">
+      <c r="N4" s="25" t="n">
         <v>0.127026032</v>
       </c>
-      <c r="O4" s="24" t="n">
+      <c r="O4" s="25" t="n">
         <v>7.1641</v>
       </c>
-      <c r="P4" s="24" t="n">
+      <c r="P4" s="25" t="n">
         <v>0.151140665</v>
       </c>
-      <c r="Q4" s="24" t="n">
+      <c r="Q4" s="25" t="n">
         <v>8.3935</v>
       </c>
-      <c r="R4" s="24" t="n">
+      <c r="R4" s="25" t="n">
         <v>-630177.7442</v>
       </c>
-      <c r="S4" s="24" t="n">
+      <c r="S4" s="25" t="n">
         <v>683001.4427</v>
       </c>
-      <c r="T4" s="24" t="n">
+      <c r="T4" s="25" t="n">
         <v>317.1813</v>
       </c>
-      <c r="U4" s="24" t="n">
+      <c r="U4" s="25" t="n">
         <v>5.537992742</v>
       </c>
-      <c r="V4" s="24" t="n">
+      <c r="V4" s="25" t="n">
         <v>324.3454</v>
       </c>
-      <c r="W4" s="24" t="n">
+      <c r="W4" s="25" t="n">
         <v>5.665018775</v>
       </c>
-      <c r="X4" s="24" t="n">
+      <c r="X4" s="25" t="n">
         <v>325.5748</v>
       </c>
-      <c r="Y4" s="24" t="n">
+      <c r="Y4" s="25" t="n">
         <v>5.689133407</v>
       </c>
-      <c r="Z4" s="24" t="n">
+      <c r="Z4" s="25" t="n">
         <v>-709005</v>
       </c>
-      <c r="AA4" s="24" t="n">
+      <c r="AA4" s="25" t="n">
         <v>846434</v>
       </c>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AE4" s="24" t="n">
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AE4" s="25" t="n">
         <v>-709005</v>
       </c>
-      <c r="AF4" s="24" t="n">
+      <c r="AF4" s="25" t="n">
         <v>846436</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="24" t="n">
+      <c r="A5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="25" t="n">
         <v>-100000</v>
       </c>
-      <c r="C5" s="24" t="n">
+      <c r="C5" s="25" t="n">
         <v>-100000</v>
       </c>
-      <c r="D5" s="24" t="n">
+      <c r="D5" s="25" t="n">
         <v>163.0559</v>
       </c>
-      <c r="E5" s="24" t="n">
+      <c r="E5" s="25" t="n">
         <v>587159</v>
       </c>
-      <c r="F5" s="24" t="n">
+      <c r="F5" s="25" t="n">
         <v>-200000</v>
       </c>
-      <c r="G5" s="24" t="n">
+      <c r="G5" s="25" t="n">
         <v>-200000</v>
       </c>
-      <c r="H5" s="24" t="n">
+      <c r="H5" s="25" t="n">
         <v>183.5442</v>
       </c>
-      <c r="I5" s="24" t="n">
+      <c r="I5" s="25" t="n">
         <v>662082</v>
       </c>
-      <c r="J5" s="24" t="n">
+      <c r="J5" s="25" t="n">
         <v>-100000</v>
       </c>
-      <c r="K5" s="24" t="n">
+      <c r="K5" s="25" t="n">
         <v>-300000</v>
       </c>
-      <c r="L5" s="24" t="n">
+      <c r="L5" s="25" t="n">
         <v>206.2045</v>
       </c>
-      <c r="M5" s="24" t="n">
+      <c r="M5" s="25" t="n">
         <v>742845</v>
       </c>
-      <c r="N5" s="24" t="n">
+      <c r="N5" s="25" t="n">
         <v>0.363236954</v>
       </c>
-      <c r="O5" s="24" t="n">
+      <c r="O5" s="25" t="n">
         <v>20.4843</v>
       </c>
-      <c r="P5" s="24" t="n">
+      <c r="P5" s="25" t="n">
         <v>0.754787027</v>
       </c>
-      <c r="Q5" s="24" t="n">
+      <c r="Q5" s="25" t="n">
         <v>43.1446</v>
       </c>
-      <c r="R5" s="24" t="n">
+      <c r="R5" s="25" t="n">
         <v>49548.54946</v>
       </c>
-      <c r="S5" s="24" t="n">
+      <c r="S5" s="25" t="n">
         <v>-163086.6288</v>
       </c>
-      <c r="T5" s="24" t="n">
+      <c r="T5" s="25" t="n">
         <v>163.0601</v>
       </c>
-      <c r="U5" s="24" t="n">
+      <c r="U5" s="25" t="n">
         <v>2.846636858</v>
       </c>
-      <c r="V5" s="24" t="n">
+      <c r="V5" s="25" t="n">
         <v>183.5444</v>
       </c>
-      <c r="W5" s="24" t="n">
+      <c r="W5" s="25" t="n">
         <v>3.209873812</v>
       </c>
-      <c r="X5" s="24" t="n">
+      <c r="X5" s="25" t="n">
         <v>206.2047</v>
       </c>
-      <c r="Y5" s="24" t="n">
+      <c r="Y5" s="25" t="n">
         <v>3.601423886</v>
       </c>
-      <c r="Z5" s="24" t="n">
+      <c r="Z5" s="25" t="n">
         <v>150295</v>
       </c>
-      <c r="AA5" s="24" t="n">
+      <c r="AA5" s="25" t="n">
         <v>-176044</v>
       </c>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AE5" s="24" t="n">
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AE5" s="25" t="n">
         <v>150295</v>
       </c>
-      <c r="AF5" s="24" t="n">
+      <c r="AF5" s="25" t="n">
         <v>-176044</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="24"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="24"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="25"/>
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="24"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="25"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="24"/>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="24"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="24"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="24"/>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="24"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="25"/>
+      <c r="AC11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="24"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="25"/>
+      <c r="AC12" s="25"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
-      <c r="U13" s="24"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24"/>
-      <c r="AA13" s="24"/>
-      <c r="AB13" s="24"/>
-      <c r="AC13" s="24"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="25"/>
+      <c r="AB13" s="25"/>
+      <c r="AC13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="24"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="25"/>
+      <c r="AA14" s="25"/>
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="25"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+      <c r="Y15" s="25"/>
+      <c r="Z15" s="25"/>
+      <c r="AA15" s="25"/>
+      <c r="AB15" s="25"/>
+      <c r="AC15" s="25"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="24"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
+      <c r="AA16" s="25"/>
+      <c r="AB16" s="25"/>
+      <c r="AC16" s="25"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="24"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="25"/>
+      <c r="AC17" s="25"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="25"/>
+      <c r="X18" s="25"/>
+      <c r="Y18" s="25"/>
+      <c r="Z18" s="25"/>
+      <c r="AA18" s="25"/>
+      <c r="AB18" s="25"/>
+      <c r="AC18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
+      <c r="V19" s="25"/>
+      <c r="W19" s="25"/>
+      <c r="X19" s="25"/>
+      <c r="Y19" s="25"/>
+      <c r="Z19" s="25"/>
+      <c r="AA19" s="25"/>
+      <c r="AB19" s="25"/>
+      <c r="AC19" s="25"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
+      <c r="AA20" s="25"/>
+      <c r="AB20" s="25"/>
+      <c r="AC20" s="25"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="24"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="25"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
+      <c r="Y21" s="25"/>
+      <c r="Z21" s="25"/>
+      <c r="AA21" s="25"/>
+      <c r="AB21" s="25"/>
+      <c r="AC21" s="25"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G23" s="25" t="n">
+      <c r="G23" s="26" t="n">
         <v>1296000</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>69</v>
+      <c r="D24" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="26" t="n">
+      <c r="D25" s="27" t="n">
         <v>1265914</v>
       </c>
-      <c r="E25" s="26" t="n">
+      <c r="E25" s="27" t="n">
         <v>62348</v>
       </c>
-      <c r="F25" s="26" t="n">
+      <c r="F25" s="27" t="n">
         <v>92434</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="26" t="n">
+      <c r="D26" s="27" t="n">
         <v>62348</v>
       </c>
-      <c r="E26" s="26" t="n">
+      <c r="E26" s="27" t="n">
         <v>1265914</v>
       </c>
-      <c r="F26" s="26" t="n">
+      <c r="F26" s="27" t="n">
         <v>1203566</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="26" t="n">
+      <c r="D27" s="27" t="n">
         <v>1142287</v>
       </c>
-      <c r="E27" s="26" t="n">
+      <c r="E27" s="27" t="n">
         <v>587159</v>
       </c>
-      <c r="F27" s="26" t="n">
+      <c r="F27" s="27" t="n">
         <v>740872</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="26" t="n">
+      <c r="D28" s="27" t="n">
         <v>587159</v>
       </c>
-      <c r="E28" s="26" t="n">
+      <c r="E28" s="27" t="n">
         <v>1142287</v>
       </c>
-      <c r="F28" s="26" t="n">
+      <c r="F28" s="27" t="n">
         <v>555128</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2292,7 +2311,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2305,145 +2324,145 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="E1" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="H1" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="I1" s="29" t="s">
         <v>79</v>
       </c>
+      <c r="J1" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="n">
+      <c r="A2" s="30" t="n">
         <v>1000000000</v>
       </c>
-      <c r="B2" s="29" t="n">
+      <c r="B2" s="30" t="n">
         <v>1000000000</v>
       </c>
-      <c r="C2" s="29" t="n">
+      <c r="C2" s="30" t="n">
         <v>100000</v>
       </c>
-      <c r="D2" s="29" t="n">
+      <c r="D2" s="30" t="n">
         <v>2000000000</v>
       </c>
-      <c r="E2" s="29" t="n">
+      <c r="E2" s="30" t="n">
         <v>2000000000</v>
       </c>
-      <c r="F2" s="29" t="n">
+      <c r="F2" s="30" t="n">
         <v>200000</v>
       </c>
-      <c r="G2" s="29" t="n">
+      <c r="G2" s="30" t="n">
         <v>162000</v>
       </c>
-      <c r="H2" s="29" t="n">
+      <c r="H2" s="30" t="n">
         <v>1414213562</v>
       </c>
-      <c r="I2" s="29" t="n">
+      <c r="I2" s="30" t="n">
         <v>1414213566</v>
       </c>
-      <c r="J2" s="29" t="n">
+      <c r="J2" s="30" t="n">
         <v>14</v>
       </c>
-      <c r="K2" s="29" t="n">
+      <c r="K2" s="30" t="n">
         <v>100000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="n">
+      <c r="A3" s="30" t="n">
         <v>2000000000</v>
       </c>
-      <c r="B3" s="29" t="n">
+      <c r="B3" s="30" t="n">
         <v>2000000000</v>
       </c>
-      <c r="C3" s="29" t="n">
+      <c r="C3" s="30" t="n">
         <v>200000</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Feat: developed integration tests for PotenotServiceImpl and testing endpoint geocalculator/potenot
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">PotenotTask*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PotenotServiseImplIntegrationtrest, ручное тестирование geocalculator/potenot</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -673,7 +676,7 @@
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -1051,10 +1054,18 @@
       <c r="E25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
+      <c r="A26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="6" t="n">
+        <v>45693</v>
+      </c>
+      <c r="C26" s="7" t="n">
+        <v>0.0520833333333333</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="E26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,7 +1077,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="13" t="n">
@@ -1092,7 +1103,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -1101,22 +1112,22 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C32" s="7" t="n">
         <v>0.0416666666666667</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33" s="16" t="n">
         <v>45678</v>
@@ -1125,13 +1136,13 @@
         <v>0.0277777777777778</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B34" s="16" t="n">
         <v>45679</v>
@@ -1140,7 +1151,7 @@
         <v>0.0381944444444444</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1221,7 +1232,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1247,96 +1258,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>47</v>
-      </c>
       <c r="J1" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="23" t="s">
-        <v>55</v>
-      </c>
       <c r="R1" s="23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S1" s="23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T1" s="23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U1" s="23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="W1" s="23" t="s">
-        <v>60</v>
-      </c>
       <c r="X1" s="23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Y1" s="23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z1" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AA1" s="24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AB1" s="24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AC1" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>100000</v>
@@ -1427,7 +1438,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B3" s="25" t="n">
         <v>100000</v>
@@ -1518,7 +1529,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="25" t="n">
         <v>100000</v>
@@ -1609,7 +1620,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="25" t="n">
         <v>-100000</v>
@@ -2201,13 +2212,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,7 +2322,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2325,37 +2336,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Work: developed and tested InverseValidator, DirectValidator, PotenotValidator
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t xml:space="preserve">PotenotServiseImplIntegrationtrest, ручное тестирование geocalculator/potenot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InverseValidator, DirectValidator, PotenotValidator разработка и тесты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validator</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -670,13 +676,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -1069,23 +1075,26 @@
       <c r="E26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
+      <c r="A27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="6" t="n">
+        <v>45694</v>
+      </c>
+      <c r="C27" s="7" t="n">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="E27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13" t="n">
-        <f aca="false">SUM(C3:C24)</f>
-        <v>1.86805555555556</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="11"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
@@ -1102,78 +1111,83 @@
       <c r="E30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
+      <c r="A31" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13" t="n">
+        <f aca="false">SUM(C3:C24)</f>
+        <v>1.86805555555556</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="7" t="n">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="7" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="16" t="n">
+      <c r="D35" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="16" t="n">
         <v>45678</v>
       </c>
-      <c r="C33" s="7" t="n">
+      <c r="C36" s="7" t="n">
         <v>0.0277777777777778</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
+      <c r="D36" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="16" t="n">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="16" t="n">
         <v>45679</v>
       </c>
-      <c r="C34" s="7" t="n">
+      <c r="C37" s="7" t="n">
         <v>0.0381944444444444</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="E37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,25 +1205,46 @@
       <c r="E39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="17"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="17"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="20"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="20"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="20"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="17"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="20"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="20"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A34:E34"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1232,7 +1267,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1258,96 +1293,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G1" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>48</v>
-      </c>
       <c r="J1" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q1" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S1" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="T1" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="U1" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="V1" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="W1" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="X1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="Y1" s="23" t="s">
-        <v>61</v>
-      </c>
       <c r="Z1" s="24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AA1" s="24" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AB1" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AC1" s="24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>100000</v>
@@ -1438,7 +1473,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="25" t="n">
         <v>100000</v>
@@ -1529,7 +1564,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="25" t="n">
         <v>100000</v>
@@ -1620,7 +1655,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B5" s="25" t="n">
         <v>-100000</v>
@@ -2212,13 +2247,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2357,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2336,37 +2371,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Feat: add validation raw data to UiController and has maked test for all end-points
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t xml:space="preserve">Validator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UiController: внедрена валидация и протестированы postman все end-points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uicontroller</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -679,10 +685,10 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -1090,10 +1096,18 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
+      <c r="A28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="6" t="n">
+        <v>45695</v>
+      </c>
+      <c r="C28" s="7" t="n">
+        <v>0.118055555555556</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,7 +1126,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="13" t="n">
@@ -1138,7 +1152,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1147,22 +1161,22 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C35" s="7" t="n">
         <v>0.0416666666666667</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B36" s="16" t="n">
         <v>45678</v>
@@ -1171,13 +1185,13 @@
         <v>0.0277777777777778</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B37" s="16" t="n">
         <v>45679</v>
@@ -1186,7 +1200,7 @@
         <v>0.0381944444444444</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1267,7 +1281,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1293,96 +1307,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G1" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>50</v>
-      </c>
       <c r="J1" s="22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="S1" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="T1" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="U1" s="23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="V1" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="W1" s="23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="X1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="Y1" s="23" t="s">
-        <v>63</v>
-      </c>
       <c r="Z1" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AA1" s="24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AB1" s="24" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AC1" s="24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>100000</v>
@@ -1473,7 +1487,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3" s="25" t="n">
         <v>100000</v>
@@ -1564,7 +1578,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B4" s="25" t="n">
         <v>100000</v>
@@ -1655,7 +1669,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B5" s="25" t="n">
         <v>-100000</v>
@@ -2247,13 +2261,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="27" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2357,7 +2371,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2371,37 +2385,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Work: updates views templates
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t xml:space="preserve">Uicontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Работа над макетами views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tamplates/*</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -684,11 +690,11 @@
   </sheetPr>
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -1111,10 +1117,18 @@
       <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
+      <c r="A29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="6" t="n">
+        <v>45698</v>
+      </c>
+      <c r="C29" s="7" t="n">
+        <v>0.0208333333333333</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,7 +1140,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="13" t="n">
@@ -1152,7 +1166,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1161,22 +1175,22 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C35" s="7" t="n">
         <v>0.0416666666666667</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B36" s="16" t="n">
         <v>45678</v>
@@ -1185,13 +1199,13 @@
         <v>0.0277777777777778</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B37" s="16" t="n">
         <v>45679</v>
@@ -1200,7 +1214,7 @@
         <v>0.0381944444444444</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1281,7 +1295,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -1307,96 +1321,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>52</v>
-      </c>
       <c r="J1" s="22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Q1" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="S1" s="23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T1" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="U1" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="V1" s="23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="W1" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="X1" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="23" t="s">
-        <v>65</v>
-      </c>
       <c r="Z1" s="24" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AA1" s="24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AB1" s="24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AC1" s="24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>100000</v>
@@ -1487,7 +1501,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" s="25" t="n">
         <v>100000</v>
@@ -1578,7 +1592,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B4" s="25" t="n">
         <v>100000</v>
@@ -1669,7 +1683,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" s="25" t="n">
         <v>-100000</v>
@@ -2261,13 +2275,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,7 +2385,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2385,37 +2399,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>